<commit_message>
analysing number of folowwers on twitter and the number of subscriber in newsletter
</commit_message>
<xml_diff>
--- a/Data Analysis - Introducao a series temporais e analises/Fundamentos Data Analysis 1 - Alura.xlsx
+++ b/Data Analysis - Introducao a series temporais e analises/Fundamentos Data Analysis 1 - Alura.xlsx
@@ -3,7 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Fundamentos Data Analysis 1 - E" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Vendas por Mês" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Assinantes Newsletter" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Seguidores Twitter" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,9 +13,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Mês</t>
+  </si>
+  <si>
+    <t>Seguidores no Twitter</t>
+  </si>
+  <si>
+    <t>Assinatura Newsletter</t>
+  </si>
+  <si>
+    <t>Aumento no número de assinantes</t>
+  </si>
+  <si>
+    <t>Aumento dos seguidores no Twitter</t>
+  </si>
+  <si>
+    <t>Aceleração no número de assinantes</t>
+  </si>
+  <si>
+    <t>Aceleração dos seguidores no Twitter</t>
   </si>
   <si>
     <t>Vendas em mil R$</t>
@@ -35,7 +55,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d&quot;-&quot;mmm&quot;-&quot;yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -43,6 +63,13 @@
     </font>
     <font>
       <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <name val="Arial"/>
     </font>
     <font/>
   </fonts>
@@ -60,20 +87,32 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -113,7 +152,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Fundamentos Data Analysis 1 - E'!$B$1</c:f>
+              <c:f>'Vendas por Mês'!$B$1</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -128,21 +167,21 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Fundamentos Data Analysis 1 - E'!$A$2:$A$25</c:f>
+              <c:f>'Vendas por Mês'!$A$2:$A$25</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Fundamentos Data Analysis 1 - E'!$B$2:$B$25</c:f>
+              <c:f>'Vendas por Mês'!$B$2:$B$25</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1461856248"/>
-        <c:axId val="554401443"/>
+        <c:axId val="1486166207"/>
+        <c:axId val="1052934806"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1461856248"/>
+        <c:axId val="1486166207"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -174,10 +213,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="554401443"/>
+        <c:crossAx val="1052934806"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="554401443"/>
+        <c:axId val="1052934806"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -225,7 +264,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1461856248"/>
+        <c:crossAx val="1486166207"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -266,7 +305,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Fundamentos Data Analysis 1 - E'!$C$1</c:f>
+              <c:f>'Vendas por Mês'!$C$1</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -281,16 +320,16 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Fundamentos Data Analysis 1 - E'!$C$2:$C$24</c:f>
+              <c:f>'Vendas por Mês'!$C$2:$C$24</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1541625215"/>
-        <c:axId val="649027393"/>
+        <c:axId val="1648159081"/>
+        <c:axId val="1268754403"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1541625215"/>
+        <c:axId val="1648159081"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -322,10 +361,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="649027393"/>
+        <c:crossAx val="1268754403"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="649027393"/>
+        <c:axId val="1268754403"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -373,7 +412,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1541625215"/>
+        <c:crossAx val="1648159081"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -414,7 +453,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Fundamentos Data Analysis 1 - E'!$D$1</c:f>
+              <c:f>'Vendas por Mês'!$D$1</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -429,16 +468,16 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Fundamentos Data Analysis 1 - E'!$D$2:$D$23</c:f>
+              <c:f>'Vendas por Mês'!$D$2:$D$23</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1167419702"/>
-        <c:axId val="2125442581"/>
+        <c:axId val="966257933"/>
+        <c:axId val="423559127"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1167419702"/>
+        <c:axId val="966257933"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -453,10 +492,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125442581"/>
+        <c:crossAx val="423559127"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125442581"/>
+        <c:axId val="423559127"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -504,7 +543,905 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1167419702"/>
+        <c:crossAx val="966257933"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Assinantes da Newsletter por mês</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Assinantes Newsletter'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Assinantes Newsletter'!$A$2:$A$25</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Assinantes Newsletter'!$B$2:$B$25</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="226665248"/>
+        <c:axId val="1965864138"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="226665248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Tempo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1965864138"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1965864138"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Total de Assinantes da Newsletter</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226665248"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Aumento no número de assinantes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Assinantes Newsletter'!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Assinantes Newsletter'!$C$2:$C$24</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="329011583"/>
+        <c:axId val="1732654794"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="329011583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Tempo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1732654794"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1732654794"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Aumento No Assinantes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="329011583"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Aceleração no número de assinantes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Assinantes Newsletter'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Assinantes Newsletter'!$D$2:$D$23</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="496030285"/>
+        <c:axId val="755942207"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="496030285"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Tempo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="755942207"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="755942207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Aceleração No Assinantes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="496030285"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Seguidores no Twitter por Mês</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Seguidores Twitter'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Seguidores Twitter'!$A$2:$A$25</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Seguidores Twitter'!$B$2:$B$25</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1209211566"/>
+        <c:axId val="1058956488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1209211566"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Tempo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1058956488"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1058956488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Seguidores no Twitter</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1209211566"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Aumento dos seguidores no Twitter</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Seguidores Twitter'!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Seguidores Twitter'!$C$2:$C$24</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="2111895292"/>
+        <c:axId val="774451405"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2111895292"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Tempo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="774451405"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="774451405"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Aumento No Seguidores Twitter</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2111895292"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Aceleração dos seguidores no Twitter</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Seguidores Twitter'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Seguidores Twitter'!$D$2:$D$23</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="725822081"/>
+        <c:axId val="2125732673"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="725822081"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Tempo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2125732673"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2125732673"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Aceleração No seguidores Twitter</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="725822081"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -528,7 +1465,7 @@
     <xdr:ext cx="6105525" cy="2171700"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1" title="Gráfico"/>
+        <xdr:cNvPr id="3" name="Chart 3" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -553,7 +1490,7 @@
     <xdr:ext cx="6115050" cy="2600325"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2" title="Gráfico"/>
+        <xdr:cNvPr id="5" name="Chart 5" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -578,7 +1515,167 @@
     <xdr:ext cx="6143625" cy="2543175"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Gráfico"/>
+        <xdr:cNvPr id="8" name="Chart 8" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7696200" cy="3076575"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7762875" cy="2905125"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 5" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7820025" cy="2495550"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 7" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7191375" cy="2705100"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name="Chart 1" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7029450" cy="2743200"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 4" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7143750" cy="2847975"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 6" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -611,24 +1708,24 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="B1" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="4">
+      <c r="A2" s="8">
         <v>41640.0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="9">
         <v>10.0</v>
       </c>
       <c r="C2">
@@ -641,10 +1738,10 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="8">
         <v>41671.0</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="9">
         <v>20.0</v>
       </c>
       <c r="C3">
@@ -657,10 +1754,10 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="4">
+      <c r="A4" s="8">
         <v>41699.0</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="9">
         <v>33.0</v>
       </c>
       <c r="C4">
@@ -673,10 +1770,10 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="4">
+      <c r="A5" s="8">
         <v>41730.0</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="9">
         <v>47.0</v>
       </c>
       <c r="C5">
@@ -689,10 +1786,10 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="4">
+      <c r="A6" s="8">
         <v>41760.0</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="9">
         <v>63.0</v>
       </c>
       <c r="C6">
@@ -705,10 +1802,10 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="4">
+      <c r="A7" s="8">
         <v>41791.0</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="9">
         <v>81.0</v>
       </c>
       <c r="C7">
@@ -721,10 +1818,10 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <v>41821.0</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="9">
         <v>101.0</v>
       </c>
       <c r="C8">
@@ -737,10 +1834,10 @@
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="4">
+      <c r="A9" s="8">
         <v>41852.0</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="9">
         <v>124.0</v>
       </c>
       <c r="C9">
@@ -753,10 +1850,10 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="4">
+      <c r="A10" s="8">
         <v>41883.0</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="9">
         <v>148.0</v>
       </c>
       <c r="C10">
@@ -769,10 +1866,10 @@
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="4">
+      <c r="A11" s="8">
         <v>41913.0</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="9">
         <v>174.0</v>
       </c>
       <c r="C11">
@@ -785,10 +1882,10 @@
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="4">
+      <c r="A12" s="8">
         <v>41944.0</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="9">
         <v>201.0</v>
       </c>
       <c r="C12">
@@ -801,10 +1898,10 @@
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="4">
+      <c r="A13" s="8">
         <v>41974.0</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="9">
         <v>230.0</v>
       </c>
       <c r="C13">
@@ -817,10 +1914,10 @@
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="4">
+      <c r="A14" s="8">
         <v>42005.0</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="9">
         <v>261.0</v>
       </c>
       <c r="C14">
@@ -833,10 +1930,10 @@
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="4">
+      <c r="A15" s="8">
         <v>42036.0</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="9">
         <v>293.0</v>
       </c>
       <c r="C15">
@@ -849,10 +1946,10 @@
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="4">
+      <c r="A16" s="8">
         <v>42064.0</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="9">
         <v>326.0</v>
       </c>
       <c r="C16">
@@ -865,10 +1962,10 @@
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="4">
+      <c r="A17" s="8">
         <v>42095.0</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="9">
         <v>362.0</v>
       </c>
       <c r="C17">
@@ -881,10 +1978,10 @@
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="4">
+      <c r="A18" s="8">
         <v>42125.0</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="9">
         <v>400.0</v>
       </c>
       <c r="C18">
@@ -897,10 +1994,10 @@
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="4">
+      <c r="A19" s="8">
         <v>42156.0</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="9">
         <v>440.0</v>
       </c>
       <c r="C19">
@@ -913,10 +2010,10 @@
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="4">
+      <c r="A20" s="8">
         <v>42186.0</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="9">
         <v>483.0</v>
       </c>
       <c r="C20">
@@ -929,10 +2026,10 @@
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="4">
+      <c r="A21" s="8">
         <v>42217.0</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="9">
         <v>527.0</v>
       </c>
       <c r="C21">
@@ -945,10 +2042,10 @@
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="4">
+      <c r="A22" s="8">
         <v>42248.0</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="9">
         <v>573.0</v>
       </c>
       <c r="C22">
@@ -961,10 +2058,10 @@
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="4">
+      <c r="A23" s="8">
         <v>42278.0</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="9">
         <v>621.0</v>
       </c>
       <c r="C23">
@@ -975,15 +2072,15 @@
         <f t="shared" si="22"/>
         <v>2</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>4</v>
+      <c r="E23" s="10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="4">
+      <c r="A24" s="8">
         <v>42309.0</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="9">
         <v>670.0</v>
       </c>
       <c r="C24">
@@ -992,612 +2089,612 @@
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="4">
+      <c r="A25" s="8">
         <v>42339.0</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="9">
         <v>721.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="4"/>
+      <c r="A26" s="8"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="4"/>
+      <c r="A27" s="8"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="4"/>
+      <c r="A28" s="8"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="4"/>
+      <c r="A29" s="8"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="4"/>
+      <c r="A30" s="8"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="4"/>
+      <c r="A31" s="8"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="4"/>
+      <c r="A32" s="8"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="4"/>
+      <c r="A33" s="8"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="4"/>
+      <c r="A34" s="8"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="4"/>
+      <c r="A35" s="8"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="4"/>
+      <c r="A36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="4"/>
+      <c r="A37" s="8"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="4"/>
+      <c r="A38" s="8"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="4"/>
+      <c r="A39" s="8"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="4"/>
+      <c r="A40" s="8"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="4"/>
+      <c r="A41" s="8"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="4"/>
+      <c r="A42" s="8"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="4"/>
+      <c r="A43" s="8"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="4"/>
+      <c r="A44" s="8"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="4"/>
+      <c r="A45" s="8"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="4"/>
+      <c r="A46" s="8"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="4"/>
+      <c r="A47" s="8"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="4"/>
+      <c r="A48" s="8"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="4"/>
+      <c r="A49" s="8"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="4"/>
+      <c r="A50" s="8"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="4"/>
+      <c r="A51" s="8"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="4"/>
+      <c r="A52" s="8"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="4"/>
+      <c r="A53" s="8"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="4"/>
+      <c r="A54" s="8"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="4"/>
+      <c r="A55" s="8"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="4"/>
+      <c r="A56" s="8"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="4"/>
+      <c r="A57" s="8"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="4"/>
+      <c r="A58" s="8"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="4"/>
+      <c r="A59" s="8"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="4"/>
+      <c r="A60" s="8"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="4"/>
+      <c r="A61" s="8"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="4"/>
+      <c r="A62" s="8"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="4"/>
+      <c r="A63" s="8"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="4"/>
+      <c r="A64" s="8"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="4"/>
+      <c r="A65" s="8"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="4"/>
+      <c r="A66" s="8"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="4"/>
+      <c r="A67" s="8"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="4"/>
+      <c r="A68" s="8"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="4"/>
+      <c r="A69" s="8"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="4"/>
+      <c r="A70" s="8"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="4"/>
+      <c r="A71" s="8"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="4"/>
+      <c r="A72" s="8"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="4"/>
+      <c r="A73" s="8"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="4"/>
+      <c r="A74" s="8"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="4"/>
+      <c r="A75" s="8"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="4"/>
+      <c r="A76" s="8"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="4"/>
+      <c r="A77" s="8"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="4"/>
+      <c r="A78" s="8"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="4"/>
+      <c r="A79" s="8"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="4"/>
+      <c r="A80" s="8"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="4"/>
+      <c r="A81" s="8"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="4"/>
+      <c r="A82" s="8"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="4"/>
+      <c r="A83" s="8"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="4"/>
+      <c r="A84" s="8"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="4"/>
+      <c r="A85" s="8"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="4"/>
+      <c r="A86" s="8"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="4"/>
+      <c r="A87" s="8"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="4"/>
+      <c r="A88" s="8"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="4"/>
+      <c r="A89" s="8"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="4"/>
+      <c r="A90" s="8"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="4"/>
+      <c r="A91" s="8"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="4"/>
+      <c r="A92" s="8"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="4"/>
+      <c r="A93" s="8"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="4"/>
+      <c r="A94" s="8"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="4"/>
+      <c r="A95" s="8"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="4"/>
+      <c r="A96" s="8"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="4"/>
+      <c r="A97" s="8"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="4"/>
+      <c r="A98" s="8"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="4"/>
+      <c r="A99" s="8"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="4"/>
+      <c r="A100" s="8"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="4"/>
+      <c r="A101" s="8"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="4"/>
+      <c r="A102" s="8"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="4"/>
+      <c r="A103" s="8"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="4"/>
+      <c r="A104" s="8"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="4"/>
+      <c r="A105" s="8"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="4"/>
+      <c r="A106" s="8"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="4"/>
+      <c r="A107" s="8"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="4"/>
+      <c r="A108" s="8"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="4"/>
+      <c r="A109" s="8"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="4"/>
+      <c r="A110" s="8"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="4"/>
+      <c r="A111" s="8"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="4"/>
+      <c r="A112" s="8"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="4"/>
+      <c r="A113" s="8"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="4"/>
+      <c r="A114" s="8"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="4"/>
+      <c r="A115" s="8"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="4"/>
+      <c r="A116" s="8"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="4"/>
+      <c r="A117" s="8"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="4"/>
+      <c r="A118" s="8"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="4"/>
+      <c r="A119" s="8"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="4"/>
+      <c r="A120" s="8"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="4"/>
+      <c r="A121" s="8"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="4"/>
+      <c r="A122" s="8"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="4"/>
+      <c r="A123" s="8"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="4"/>
+      <c r="A124" s="8"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="4"/>
+      <c r="A125" s="8"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="4"/>
+      <c r="A126" s="8"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="4"/>
+      <c r="A127" s="8"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="4"/>
+      <c r="A128" s="8"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="4"/>
+      <c r="A129" s="8"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="4"/>
+      <c r="A130" s="8"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="4"/>
+      <c r="A131" s="8"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="4"/>
+      <c r="A132" s="8"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="4"/>
+      <c r="A133" s="8"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="4"/>
+      <c r="A134" s="8"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="4"/>
+      <c r="A135" s="8"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="4"/>
+      <c r="A136" s="8"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="4"/>
+      <c r="A137" s="8"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="4"/>
+      <c r="A138" s="8"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="4"/>
+      <c r="A139" s="8"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="4"/>
+      <c r="A140" s="8"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="4"/>
+      <c r="A141" s="8"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="4"/>
+      <c r="A142" s="8"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="4"/>
+      <c r="A143" s="8"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="4"/>
+      <c r="A144" s="8"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="4"/>
+      <c r="A145" s="8"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="4"/>
+      <c r="A146" s="8"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="4"/>
+      <c r="A147" s="8"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="4"/>
+      <c r="A148" s="8"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="4"/>
+      <c r="A149" s="8"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="4"/>
+      <c r="A150" s="8"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="4"/>
+      <c r="A151" s="8"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="4"/>
+      <c r="A152" s="8"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="4"/>
+      <c r="A153" s="8"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="4"/>
+      <c r="A154" s="8"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="4"/>
+      <c r="A155" s="8"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="4"/>
+      <c r="A156" s="8"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="4"/>
+      <c r="A157" s="8"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="4"/>
+      <c r="A158" s="8"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="4"/>
+      <c r="A159" s="8"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="4"/>
+      <c r="A160" s="8"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="4"/>
+      <c r="A161" s="8"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="4"/>
+      <c r="A162" s="8"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="4"/>
+      <c r="A163" s="8"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="4"/>
+      <c r="A164" s="8"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="4"/>
+      <c r="A165" s="8"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="4"/>
+      <c r="A166" s="8"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="4"/>
+      <c r="A167" s="8"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="4"/>
+      <c r="A168" s="8"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="4"/>
+      <c r="A169" s="8"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="4"/>
+      <c r="A170" s="8"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="4"/>
+      <c r="A171" s="8"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="4"/>
+      <c r="A172" s="8"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="4"/>
+      <c r="A173" s="8"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="4"/>
+      <c r="A174" s="8"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="4"/>
+      <c r="A175" s="8"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="4"/>
+      <c r="A176" s="8"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="4"/>
+      <c r="A177" s="8"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="4"/>
+      <c r="A178" s="8"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="4"/>
+      <c r="A179" s="8"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="4"/>
+      <c r="A180" s="8"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="A181" s="4"/>
+      <c r="A181" s="8"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="A182" s="4"/>
+      <c r="A182" s="8"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="4"/>
+      <c r="A183" s="8"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="4"/>
+      <c r="A184" s="8"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="4"/>
+      <c r="A185" s="8"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="4"/>
+      <c r="A186" s="8"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="A187" s="4"/>
+      <c r="A187" s="8"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="A188" s="4"/>
+      <c r="A188" s="8"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="A189" s="4"/>
+      <c r="A189" s="8"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="A190" s="4"/>
+      <c r="A190" s="8"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="A191" s="4"/>
+      <c r="A191" s="8"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="A192" s="4"/>
+      <c r="A192" s="8"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="4"/>
+      <c r="A193" s="8"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="4"/>
+      <c r="A194" s="8"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="4"/>
+      <c r="A195" s="8"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="4"/>
+      <c r="A196" s="8"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="4"/>
+      <c r="A197" s="8"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="4"/>
+      <c r="A198" s="8"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="4"/>
+      <c r="A199" s="8"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="4"/>
+      <c r="A200" s="8"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="4"/>
+      <c r="A201" s="8"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="4"/>
+      <c r="A202" s="8"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="4"/>
+      <c r="A203" s="8"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="4"/>
+      <c r="A204" s="8"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="4"/>
+      <c r="A205" s="8"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="4"/>
+      <c r="A206" s="8"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="4"/>
+      <c r="A207" s="8"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="4"/>
+      <c r="A208" s="8"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="4"/>
+      <c r="A209" s="8"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="4"/>
+      <c r="A210" s="8"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="4"/>
+      <c r="A211" s="8"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="4"/>
+      <c r="A212" s="8"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="4"/>
+      <c r="A213" s="8"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="4"/>
+      <c r="A214" s="8"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="4"/>
+      <c r="A215" s="8"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="4"/>
+      <c r="A216" s="8"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="4"/>
+      <c r="A217" s="8"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="4"/>
+      <c r="A218" s="8"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="A219" s="4"/>
+      <c r="A219" s="8"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="4"/>
+      <c r="A220" s="8"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="4"/>
+      <c r="A221" s="8"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="4"/>
+      <c r="A222" s="8"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="4"/>
+      <c r="A223" s="8"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="4"/>
+      <c r="A224" s="8"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="4"/>
+      <c r="A225" s="8"/>
     </row>
     <row r="226" ht="15.75" customHeight="1"/>
     <row r="227" ht="15.75" customHeight="1"/>
@@ -2377,4 +3474,816 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="20.71"/>
+    <col customWidth="1" min="3" max="3" width="32.14"/>
+    <col customWidth="1" min="4" max="4" width="34.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4">
+        <v>41640.0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:D2" si="1">B3-B2</f>
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4">
+        <v>41671.0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:D3" si="2">B4-B3</f>
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4">
+        <v>41699.0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>21.0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:D4" si="3">B5-B4</f>
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4">
+        <v>41730.0</v>
+      </c>
+      <c r="B5" s="5">
+        <v>34.0</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:D5" si="4">B6-B5</f>
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4">
+        <v>41760.0</v>
+      </c>
+      <c r="B6" s="5">
+        <v>49.0</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:D6" si="5">B7-B6</f>
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4">
+        <v>41791.0</v>
+      </c>
+      <c r="B7" s="5">
+        <v>66.0</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:D7" si="6">B8-B7</f>
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4">
+        <v>41821.0</v>
+      </c>
+      <c r="B8" s="5">
+        <v>85.0</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:D8" si="7">B9-B8</f>
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4">
+        <v>41852.0</v>
+      </c>
+      <c r="B9" s="5">
+        <v>107.0</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:D9" si="8">B10-B9</f>
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4">
+        <v>41883.0</v>
+      </c>
+      <c r="B10" s="5">
+        <v>132.0</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:D10" si="9">B11-B10</f>
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4">
+        <v>41913.0</v>
+      </c>
+      <c r="B11" s="5">
+        <v>160.0</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:D11" si="10">B12-B11</f>
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4">
+        <v>41944.0</v>
+      </c>
+      <c r="B12" s="5">
+        <v>190.0</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:D12" si="11">B13-B12</f>
+        <v>31</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4">
+        <v>41974.0</v>
+      </c>
+      <c r="B13" s="5">
+        <v>221.0</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:D13" si="12">B14-B13</f>
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4">
+        <v>42005.0</v>
+      </c>
+      <c r="B14" s="5">
+        <v>252.0</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:D14" si="13">B15-B14</f>
+        <v>31</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="13"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4">
+        <v>42036.0</v>
+      </c>
+      <c r="B15" s="5">
+        <v>283.0</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:D15" si="14">B16-B15</f>
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="14"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4">
+        <v>42064.0</v>
+      </c>
+      <c r="B16" s="5">
+        <v>313.0</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:D16" si="15">B17-B16</f>
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="15"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4">
+        <v>42095.0</v>
+      </c>
+      <c r="B17" s="5">
+        <v>341.0</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:D17" si="16">B18-B17</f>
+        <v>26</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="16"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4">
+        <v>42125.0</v>
+      </c>
+      <c r="B18" s="5">
+        <v>367.0</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:D18" si="17">B19-B18</f>
+        <v>23</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="17"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4">
+        <v>42156.0</v>
+      </c>
+      <c r="B19" s="5">
+        <v>390.0</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:D19" si="18">B20-B19</f>
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="18"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4">
+        <v>42186.0</v>
+      </c>
+      <c r="B20" s="5">
+        <v>410.0</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:D20" si="19">B21-B20</f>
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="19"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4">
+        <v>42217.0</v>
+      </c>
+      <c r="B21" s="5">
+        <v>426.0</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:D21" si="20">B22-B21</f>
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="20"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4">
+        <v>42248.0</v>
+      </c>
+      <c r="B22" s="5">
+        <v>437.0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:D22" si="21">B23-B22</f>
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="21"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4">
+        <v>42278.0</v>
+      </c>
+      <c r="B23" s="5">
+        <v>444.0</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:D23" si="22">B24-B23</f>
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4">
+        <v>42309.0</v>
+      </c>
+      <c r="B24" s="5">
+        <v>449.0</v>
+      </c>
+      <c r="C24">
+        <f>B25-B24</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4">
+        <v>42339.0</v>
+      </c>
+      <c r="B25" s="5">
+        <v>454.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="20.57"/>
+    <col customWidth="1" min="3" max="3" width="32.71"/>
+    <col customWidth="1" min="4" max="4" width="34.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4">
+        <v>41640.0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:D2" si="1">B3-B2</f>
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4">
+        <v>41671.0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:D3" si="2">B4-B3</f>
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4">
+        <v>41699.0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:D4" si="3">B5-B4</f>
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="3"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4">
+        <v>41730.0</v>
+      </c>
+      <c r="B5" s="5">
+        <v>19.0</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:D5" si="4">B6-B5</f>
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4">
+        <v>41760.0</v>
+      </c>
+      <c r="B6" s="5">
+        <v>24.0</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:D6" si="5">B7-B6</f>
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="5"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4">
+        <v>41791.0</v>
+      </c>
+      <c r="B7" s="5">
+        <v>29.0</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:D7" si="6">B8-B7</f>
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4">
+        <v>41821.0</v>
+      </c>
+      <c r="B8" s="5">
+        <v>31.0</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:D8" si="7">B9-B8</f>
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4">
+        <v>41852.0</v>
+      </c>
+      <c r="B9" s="5">
+        <v>37.0</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:D9" si="8">B10-B9</f>
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4">
+        <v>41883.0</v>
+      </c>
+      <c r="B10" s="5">
+        <v>47.0</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:D10" si="9">B11-B10</f>
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4">
+        <v>41913.0</v>
+      </c>
+      <c r="B11" s="5">
+        <v>62.0</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:D11" si="10">B12-B11</f>
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4">
+        <v>41944.0</v>
+      </c>
+      <c r="B12" s="5">
+        <v>79.0</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:D12" si="11">B13-B12</f>
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4">
+        <v>41974.0</v>
+      </c>
+      <c r="B13" s="5">
+        <v>99.0</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:D13" si="12">B14-B13</f>
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4">
+        <v>42005.0</v>
+      </c>
+      <c r="B14" s="5">
+        <v>119.0</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:D14" si="13">B15-B14</f>
+        <v>23</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4">
+        <v>42036.0</v>
+      </c>
+      <c r="B15" s="5">
+        <v>142.0</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:D15" si="14">B16-B15</f>
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="14"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4">
+        <v>42064.0</v>
+      </c>
+      <c r="B16" s="5">
+        <v>165.0</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:D16" si="15">B17-B16</f>
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4">
+        <v>42095.0</v>
+      </c>
+      <c r="B17" s="5">
+        <v>183.0</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:D17" si="16">B18-B17</f>
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4">
+        <v>42125.0</v>
+      </c>
+      <c r="B18" s="5">
+        <v>203.0</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:D18" si="17">B19-B18</f>
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="17"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4">
+        <v>42156.0</v>
+      </c>
+      <c r="B19" s="5">
+        <v>225.0</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:D19" si="18">B20-B19</f>
+        <v>19</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="18"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4">
+        <v>42186.0</v>
+      </c>
+      <c r="B20" s="5">
+        <v>244.0</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:D20" si="19">B21-B20</f>
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4">
+        <v>42217.0</v>
+      </c>
+      <c r="B21" s="5">
+        <v>262.0</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:D21" si="20">B22-B21</f>
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="20"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4">
+        <v>42248.0</v>
+      </c>
+      <c r="B22" s="5">
+        <v>282.0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:D22" si="21">B23-B22</f>
+        <v>19</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="21"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4">
+        <v>42278.0</v>
+      </c>
+      <c r="B23" s="5">
+        <v>301.0</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:D23" si="22">B24-B23</f>
+        <v>24</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4">
+        <v>42309.0</v>
+      </c>
+      <c r="B24" s="5">
+        <v>325.0</v>
+      </c>
+      <c r="C24">
+        <f>B25-B24</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4">
+        <v>42339.0</v>
+      </c>
+      <c r="B25" s="5">
+        <v>351.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
correcting amounts per working days
</commit_message>
<xml_diff>
--- a/Data Analysis - Introducao a series temporais e analises/Fundamentos Data Analysis 1 - Alura.xlsx
+++ b/Data Analysis - Introducao a series temporais e analises/Fundamentos Data Analysis 1 - Alura.xlsx
@@ -6,6 +6,8 @@
     <sheet state="visible" name="Vendas por Mês" sheetId="1" r:id="rId3"/>
     <sheet state="visible" name="Assinantes Newsletter" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="Seguidores Twitter" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="Vendas Quantidade por dia" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="Vendas em R$" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Mês</t>
   </si>
@@ -21,16 +23,7 @@
     <t>Seguidores no Twitter</t>
   </si>
   <si>
-    <t>Assinatura Newsletter</t>
-  </si>
-  <si>
-    <t>Aumento no número de assinantes</t>
-  </si>
-  <si>
     <t>Aumento dos seguidores no Twitter</t>
-  </si>
-  <si>
-    <t>Aceleração no número de assinantes</t>
   </si>
   <si>
     <t>Aceleração dos seguidores no Twitter</t>
@@ -47,13 +40,41 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>Assinatura Newsletter</t>
+  </si>
+  <si>
+    <t>Aumento no número de assinantes</t>
+  </si>
+  <si>
+    <t>Aceleração no número de assinantes</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Vendas Quantidade de produto vendido</t>
+  </si>
+  <si>
+    <t>Vendas em R$</t>
+  </si>
+  <si>
+    <t>Dias úteis</t>
+  </si>
+  <si>
+    <t>Vendas por dia útil</t>
+  </si>
+  <si>
+    <t>Aumento de Vendas por dia útil</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d&quot;-&quot;mmm&quot;-&quot;yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -87,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -100,20 +121,26 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -177,11 +204,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1486166207"/>
-        <c:axId val="1052934806"/>
+        <c:axId val="1956541801"/>
+        <c:axId val="1919053557"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1486166207"/>
+        <c:axId val="1956541801"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -213,10 +240,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1052934806"/>
+        <c:crossAx val="1919053557"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1052934806"/>
+        <c:axId val="1919053557"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -264,7 +291,609 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1486166207"/>
+        <c:crossAx val="1956541801"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Vendas em Quantidade por dia</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Vendas Quantidade por dia'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Vendas Quantidade por dia'!$A$2:$A$60</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Vendas Quantidade por dia'!$B$2:$B$60</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1958910643"/>
+        <c:axId val="1234859363"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1958910643"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Tempo (em dias)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1234859363"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1234859363"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Vendas (em quantidade de produtos)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1958910643"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Vendas em R$ por Mês</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Vendas em R$'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Vendas em R$'!$A$2:$A$25</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Vendas em R$'!$B$2:$B$25</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="413435579"/>
+        <c:axId val="980687328"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="413435579"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Mês</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="980687328"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="980687328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Vendas em R$</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="413435579"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Vendas por dia útil</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Vendas em R$'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Vendas em R$'!$D$2:$D$25</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1139149712"/>
+        <c:axId val="796959784"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1139149712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Tempo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="796959784"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="796959784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Vendas por dia útil</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1139149712"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Aumento de Vendas por dia útil</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Vendas em R$'!$E$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Vendas em R$'!$E$2:$E$24</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1536904721"/>
+        <c:axId val="1291302756"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1536904721"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Tempo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1291302756"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1291302756"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Aumento de vendas por dia útil</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1536904721"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -325,11 +954,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1648159081"/>
-        <c:axId val="1268754403"/>
+        <c:axId val="461092183"/>
+        <c:axId val="1927993042"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1648159081"/>
+        <c:axId val="461092183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -361,10 +990,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1268754403"/>
+        <c:crossAx val="1927993042"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1268754403"/>
+        <c:axId val="1927993042"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -412,7 +1041,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1648159081"/>
+        <c:crossAx val="461092183"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -473,11 +1102,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="966257933"/>
-        <c:axId val="423559127"/>
+        <c:axId val="2020559538"/>
+        <c:axId val="570560958"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="966257933"/>
+        <c:axId val="2020559538"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,10 +1121,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423559127"/>
+        <c:crossAx val="570560958"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="423559127"/>
+        <c:axId val="570560958"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -543,7 +1172,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="966257933"/>
+        <c:crossAx val="2020559538"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -609,11 +1238,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="226665248"/>
-        <c:axId val="1965864138"/>
+        <c:axId val="1714166508"/>
+        <c:axId val="1425428686"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="226665248"/>
+        <c:axId val="1714166508"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -645,10 +1274,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1965864138"/>
+        <c:crossAx val="1425428686"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1965864138"/>
+        <c:axId val="1425428686"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -696,7 +1325,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226665248"/>
+        <c:crossAx val="1714166508"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -757,11 +1386,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="329011583"/>
-        <c:axId val="1732654794"/>
+        <c:axId val="2044307724"/>
+        <c:axId val="450478907"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="329011583"/>
+        <c:axId val="2044307724"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -793,10 +1422,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1732654794"/>
+        <c:crossAx val="450478907"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1732654794"/>
+        <c:axId val="450478907"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -844,7 +1473,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329011583"/>
+        <c:crossAx val="2044307724"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -905,11 +1534,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="496030285"/>
-        <c:axId val="755942207"/>
+        <c:axId val="1353107793"/>
+        <c:axId val="810362021"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496030285"/>
+        <c:axId val="1353107793"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -941,10 +1570,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="755942207"/>
+        <c:crossAx val="810362021"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="755942207"/>
+        <c:axId val="810362021"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +1621,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496030285"/>
+        <c:crossAx val="1353107793"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1058,11 +1687,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1209211566"/>
-        <c:axId val="1058956488"/>
+        <c:axId val="392453147"/>
+        <c:axId val="1721431495"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1209211566"/>
+        <c:axId val="392453147"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1094,10 +1723,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1058956488"/>
+        <c:crossAx val="1721431495"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1058956488"/>
+        <c:axId val="1721431495"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,7 +1774,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1209211566"/>
+        <c:crossAx val="392453147"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1206,11 +1835,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2111895292"/>
-        <c:axId val="774451405"/>
+        <c:axId val="43107687"/>
+        <c:axId val="461623412"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2111895292"/>
+        <c:axId val="43107687"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,10 +1871,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="774451405"/>
+        <c:crossAx val="461623412"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="774451405"/>
+        <c:axId val="461623412"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1293,7 +1922,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2111895292"/>
+        <c:crossAx val="43107687"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1354,11 +1983,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="725822081"/>
-        <c:axId val="2125732673"/>
+        <c:axId val="1918175821"/>
+        <c:axId val="1983136492"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="725822081"/>
+        <c:axId val="1918175821"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1390,10 +2019,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125732673"/>
+        <c:crossAx val="1983136492"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125732673"/>
+        <c:axId val="1983136492"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1441,7 +2070,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="725822081"/>
+        <c:crossAx val="1918175821"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1465,7 +2094,7 @@
     <xdr:ext cx="6105525" cy="2171700"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Gráfico"/>
+        <xdr:cNvPr id="2" name="Chart 2" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1490,7 +2119,7 @@
     <xdr:ext cx="6115050" cy="2600325"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 5" title="Gráfico"/>
+        <xdr:cNvPr id="4" name="Chart 4" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1515,7 +2144,7 @@
     <xdr:ext cx="6143625" cy="2543175"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 8" title="Gráfico"/>
+        <xdr:cNvPr id="6" name="Chart 6" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1545,7 +2174,7 @@
     <xdr:ext cx="7696200" cy="3076575"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2" title="Gráfico"/>
+        <xdr:cNvPr id="1" name="Chart 1" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1595,7 +2224,7 @@
     <xdr:ext cx="7820025" cy="2495550"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 7" title="Gráfico"/>
+        <xdr:cNvPr id="8" name="Chart 8" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1650,7 +2279,7 @@
     <xdr:ext cx="7029450" cy="2743200"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 4" title="Gráfico"/>
+        <xdr:cNvPr id="3" name="Chart 3" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1675,7 +2304,117 @@
     <xdr:ext cx="7143750" cy="2847975"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 6" title="Gráfico"/>
+        <xdr:cNvPr id="7" name="Chart 7" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8724900" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 10" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7067550" cy="3362325"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 9" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7181850" cy="2790825"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 11" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7191375" cy="2800350"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 12" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1708,17 +2447,17 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>7</v>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -2073,7 +2812,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -3496,20 +4235,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <v>41640.0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="7">
         <v>0.0</v>
       </c>
       <c r="C2">
@@ -3522,10 +4261,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>41671.0</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="7">
         <v>10.0</v>
       </c>
       <c r="C3">
@@ -3538,10 +4277,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <v>41699.0</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="7">
         <v>21.0</v>
       </c>
       <c r="C4">
@@ -3554,10 +4293,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <v>41730.0</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="7">
         <v>34.0</v>
       </c>
       <c r="C5">
@@ -3570,10 +4309,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="5">
         <v>41760.0</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="7">
         <v>49.0</v>
       </c>
       <c r="C6">
@@ -3586,10 +4325,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <v>41791.0</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="7">
         <v>66.0</v>
       </c>
       <c r="C7">
@@ -3602,10 +4341,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <v>41821.0</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="7">
         <v>85.0</v>
       </c>
       <c r="C8">
@@ -3618,10 +4357,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4">
+      <c r="A9" s="5">
         <v>41852.0</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="7">
         <v>107.0</v>
       </c>
       <c r="C9">
@@ -3634,10 +4373,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4">
+      <c r="A10" s="5">
         <v>41883.0</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="7">
         <v>132.0</v>
       </c>
       <c r="C10">
@@ -3650,10 +4389,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4">
+      <c r="A11" s="5">
         <v>41913.0</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="7">
         <v>160.0</v>
       </c>
       <c r="C11">
@@ -3666,10 +4405,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4">
+      <c r="A12" s="5">
         <v>41944.0</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="7">
         <v>190.0</v>
       </c>
       <c r="C12">
@@ -3682,10 +4421,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4">
+      <c r="A13" s="5">
         <v>41974.0</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="7">
         <v>221.0</v>
       </c>
       <c r="C13">
@@ -3698,10 +4437,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4">
+      <c r="A14" s="5">
         <v>42005.0</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="7">
         <v>252.0</v>
       </c>
       <c r="C14">
@@ -3714,10 +4453,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4">
+      <c r="A15" s="5">
         <v>42036.0</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="7">
         <v>283.0</v>
       </c>
       <c r="C15">
@@ -3730,10 +4469,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4">
+      <c r="A16" s="5">
         <v>42064.0</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="7">
         <v>313.0</v>
       </c>
       <c r="C16">
@@ -3746,10 +4485,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4">
+      <c r="A17" s="5">
         <v>42095.0</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="7">
         <v>341.0</v>
       </c>
       <c r="C17">
@@ -3762,10 +4501,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4">
+      <c r="A18" s="5">
         <v>42125.0</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="7">
         <v>367.0</v>
       </c>
       <c r="C18">
@@ -3778,10 +4517,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4">
+      <c r="A19" s="5">
         <v>42156.0</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="7">
         <v>390.0</v>
       </c>
       <c r="C19">
@@ -3794,10 +4533,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4">
+      <c r="A20" s="5">
         <v>42186.0</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="7">
         <v>410.0</v>
       </c>
       <c r="C20">
@@ -3810,10 +4549,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4">
+      <c r="A21" s="5">
         <v>42217.0</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="7">
         <v>426.0</v>
       </c>
       <c r="C21">
@@ -3826,10 +4565,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4">
+      <c r="A22" s="5">
         <v>42248.0</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="7">
         <v>437.0</v>
       </c>
       <c r="C22">
@@ -3842,10 +4581,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4">
+      <c r="A23" s="5">
         <v>42278.0</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="7">
         <v>444.0</v>
       </c>
       <c r="C23">
@@ -3858,10 +4597,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4">
+      <c r="A24" s="5">
         <v>42309.0</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="7">
         <v>449.0</v>
       </c>
       <c r="C24">
@@ -3870,10 +4609,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4">
+      <c r="A25" s="5">
         <v>42339.0</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="7">
         <v>454.0</v>
       </c>
     </row>
@@ -3905,17 +4644,17 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <v>41640.0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="7">
         <v>0.0</v>
       </c>
       <c r="C2">
@@ -3928,10 +4667,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>41671.0</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="7">
         <v>5.0</v>
       </c>
       <c r="C3">
@@ -3944,10 +4683,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <v>41699.0</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="7">
         <v>11.0</v>
       </c>
       <c r="C4">
@@ -3960,10 +4699,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <v>41730.0</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="7">
         <v>19.0</v>
       </c>
       <c r="C5">
@@ -3976,10 +4715,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="5">
         <v>41760.0</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="7">
         <v>24.0</v>
       </c>
       <c r="C6">
@@ -3992,10 +4731,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <v>41791.0</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="7">
         <v>29.0</v>
       </c>
       <c r="C7">
@@ -4008,10 +4747,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <v>41821.0</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="7">
         <v>31.0</v>
       </c>
       <c r="C8">
@@ -4024,10 +4763,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4">
+      <c r="A9" s="5">
         <v>41852.0</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="7">
         <v>37.0</v>
       </c>
       <c r="C9">
@@ -4040,10 +4779,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4">
+      <c r="A10" s="5">
         <v>41883.0</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="7">
         <v>47.0</v>
       </c>
       <c r="C10">
@@ -4056,10 +4795,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4">
+      <c r="A11" s="5">
         <v>41913.0</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="7">
         <v>62.0</v>
       </c>
       <c r="C11">
@@ -4072,10 +4811,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4">
+      <c r="A12" s="5">
         <v>41944.0</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="7">
         <v>79.0</v>
       </c>
       <c r="C12">
@@ -4088,10 +4827,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4">
+      <c r="A13" s="5">
         <v>41974.0</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="7">
         <v>99.0</v>
       </c>
       <c r="C13">
@@ -4104,10 +4843,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4">
+      <c r="A14" s="5">
         <v>42005.0</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="7">
         <v>119.0</v>
       </c>
       <c r="C14">
@@ -4120,10 +4859,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4">
+      <c r="A15" s="5">
         <v>42036.0</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="7">
         <v>142.0</v>
       </c>
       <c r="C15">
@@ -4136,10 +4875,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4">
+      <c r="A16" s="5">
         <v>42064.0</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="7">
         <v>165.0</v>
       </c>
       <c r="C16">
@@ -4152,10 +4891,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4">
+      <c r="A17" s="5">
         <v>42095.0</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="7">
         <v>183.0</v>
       </c>
       <c r="C17">
@@ -4168,10 +4907,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4">
+      <c r="A18" s="5">
         <v>42125.0</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="7">
         <v>203.0</v>
       </c>
       <c r="C18">
@@ -4184,10 +4923,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4">
+      <c r="A19" s="5">
         <v>42156.0</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="7">
         <v>225.0</v>
       </c>
       <c r="C19">
@@ -4200,10 +4939,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4">
+      <c r="A20" s="5">
         <v>42186.0</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="7">
         <v>244.0</v>
       </c>
       <c r="C20">
@@ -4216,10 +4955,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4">
+      <c r="A21" s="5">
         <v>42217.0</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="7">
         <v>262.0</v>
       </c>
       <c r="C21">
@@ -4232,10 +4971,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4">
+      <c r="A22" s="5">
         <v>42248.0</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="7">
         <v>282.0</v>
       </c>
       <c r="C22">
@@ -4248,10 +4987,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4">
+      <c r="A23" s="5">
         <v>42278.0</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="7">
         <v>301.0</v>
       </c>
       <c r="C23">
@@ -4264,10 +5003,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4">
+      <c r="A24" s="5">
         <v>42309.0</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="7">
         <v>325.0</v>
       </c>
       <c r="C24">
@@ -4276,11 +5015,1002 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4">
+      <c r="A25" s="5">
         <v>42339.0</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="7">
         <v>351.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="36.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="12">
+        <v>42005.0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>51.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="12">
+        <v>42006.0</v>
+      </c>
+      <c r="B3" s="7">
+        <v>54.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="12">
+        <v>42007.0</v>
+      </c>
+      <c r="B4" s="7">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="12">
+        <v>42008.0</v>
+      </c>
+      <c r="B5" s="7">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="12">
+        <v>42009.0</v>
+      </c>
+      <c r="B6" s="7">
+        <v>57.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="12">
+        <v>42010.0</v>
+      </c>
+      <c r="B7" s="7">
+        <v>58.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="12">
+        <v>42011.0</v>
+      </c>
+      <c r="B8" s="7">
+        <v>53.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="12">
+        <v>42012.0</v>
+      </c>
+      <c r="B9" s="7">
+        <v>59.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="12">
+        <v>42013.0</v>
+      </c>
+      <c r="B10" s="7">
+        <v>58.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="12">
+        <v>42014.0</v>
+      </c>
+      <c r="B11" s="7">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="12">
+        <v>42015.0</v>
+      </c>
+      <c r="B12" s="7">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="12">
+        <v>42016.0</v>
+      </c>
+      <c r="B13" s="7">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="12">
+        <v>42017.0</v>
+      </c>
+      <c r="B14" s="7">
+        <v>56.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="12">
+        <v>42018.0</v>
+      </c>
+      <c r="B15" s="7">
+        <v>59.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="12">
+        <v>42019.0</v>
+      </c>
+      <c r="B16" s="7">
+        <v>51.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="12">
+        <v>42020.0</v>
+      </c>
+      <c r="B17" s="7">
+        <v>58.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="12">
+        <v>42021.0</v>
+      </c>
+      <c r="B18" s="7">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="12">
+        <v>42022.0</v>
+      </c>
+      <c r="B19" s="7">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="12">
+        <v>42023.0</v>
+      </c>
+      <c r="B20" s="7">
+        <v>59.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="12">
+        <v>42024.0</v>
+      </c>
+      <c r="B21" s="7">
+        <v>56.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="12">
+        <v>42025.0</v>
+      </c>
+      <c r="B22" s="7">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="12">
+        <v>42026.0</v>
+      </c>
+      <c r="B23" s="7">
+        <v>58.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="12">
+        <v>42027.0</v>
+      </c>
+      <c r="B24" s="7">
+        <v>51.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="12">
+        <v>42028.0</v>
+      </c>
+      <c r="B25" s="7">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="12">
+        <v>42029.0</v>
+      </c>
+      <c r="B26" s="7">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="12">
+        <v>42030.0</v>
+      </c>
+      <c r="B27" s="7">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="12">
+        <v>42031.0</v>
+      </c>
+      <c r="B28" s="7">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="12">
+        <v>42032.0</v>
+      </c>
+      <c r="B29" s="7">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="12">
+        <v>42033.0</v>
+      </c>
+      <c r="B30" s="7">
+        <v>53.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="12">
+        <v>42034.0</v>
+      </c>
+      <c r="B31" s="7">
+        <v>57.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="12">
+        <v>42035.0</v>
+      </c>
+      <c r="B32" s="7">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="12">
+        <v>42036.0</v>
+      </c>
+      <c r="B33" s="7">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="12">
+        <v>42037.0</v>
+      </c>
+      <c r="B34" s="7">
+        <v>58.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="12">
+        <v>42038.0</v>
+      </c>
+      <c r="B35" s="7">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="12">
+        <v>42039.0</v>
+      </c>
+      <c r="B36" s="7">
+        <v>51.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="12">
+        <v>42040.0</v>
+      </c>
+      <c r="B37" s="7">
+        <v>56.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="12">
+        <v>42041.0</v>
+      </c>
+      <c r="B38" s="7">
+        <v>51.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="12">
+        <v>42042.0</v>
+      </c>
+      <c r="B39" s="7">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="12">
+        <v>42043.0</v>
+      </c>
+      <c r="B40" s="7">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="12">
+        <v>42044.0</v>
+      </c>
+      <c r="B41" s="7">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="12">
+        <v>42045.0</v>
+      </c>
+      <c r="B42" s="7">
+        <v>53.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="12">
+        <v>42046.0</v>
+      </c>
+      <c r="B43" s="7">
+        <v>51.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="12">
+        <v>42047.0</v>
+      </c>
+      <c r="B44" s="7">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="12">
+        <v>42048.0</v>
+      </c>
+      <c r="B45" s="7">
+        <v>59.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="12">
+        <v>42049.0</v>
+      </c>
+      <c r="B46" s="7">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="12">
+        <v>42050.0</v>
+      </c>
+      <c r="B47" s="7">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="12">
+        <v>42051.0</v>
+      </c>
+      <c r="B48" s="7">
+        <v>57.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="12">
+        <v>42052.0</v>
+      </c>
+      <c r="B49" s="7">
+        <v>51.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="12">
+        <v>42053.0</v>
+      </c>
+      <c r="B50" s="7">
+        <v>54.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="12">
+        <v>42054.0</v>
+      </c>
+      <c r="B51" s="7">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="12">
+        <v>42055.0</v>
+      </c>
+      <c r="B52" s="7">
+        <v>53.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="12">
+        <v>42056.0</v>
+      </c>
+      <c r="B53" s="7">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="12">
+        <v>42057.0</v>
+      </c>
+      <c r="B54" s="7">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="12">
+        <v>42058.0</v>
+      </c>
+      <c r="B55" s="7">
+        <v>58.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="12">
+        <v>42059.0</v>
+      </c>
+      <c r="B56" s="7">
+        <v>52.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="12">
+        <v>42060.0</v>
+      </c>
+      <c r="B57" s="7">
+        <v>56.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="12">
+        <v>42061.0</v>
+      </c>
+      <c r="B58" s="7">
+        <v>56.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="12">
+        <v>42062.0</v>
+      </c>
+      <c r="B59" s="7">
+        <v>56.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="12">
+        <v>42063.0</v>
+      </c>
+      <c r="B60" s="7">
+        <v>19.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="4" max="4" width="17.71"/>
+    <col customWidth="1" min="5" max="5" width="28.86"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5">
+        <v>41640.0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>2420.0</v>
+      </c>
+      <c r="C2" s="7">
+        <v>22.0</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D25" si="1">B2/C2</f>
+        <v>110</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E24" si="2">D3-D2</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5">
+        <v>41671.0</v>
+      </c>
+      <c r="B3" s="7">
+        <v>4000.0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>20.0</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5">
+        <v>41699.0</v>
+      </c>
+      <c r="B4" s="7">
+        <v>5832.0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>18.0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>324</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5">
+        <v>41730.0</v>
+      </c>
+      <c r="B5" s="7">
+        <v>9600.0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>20.0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5">
+        <v>41760.0</v>
+      </c>
+      <c r="B6" s="7">
+        <v>13230.0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>21.0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>630</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5">
+        <v>41791.0</v>
+      </c>
+      <c r="B7" s="7">
+        <v>16400.0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>20.0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>820</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5">
+        <v>41821.0</v>
+      </c>
+      <c r="B8" s="7">
+        <v>22264.0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>22.0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>1012</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5">
+        <v>41852.0</v>
+      </c>
+      <c r="B9" s="7">
+        <v>26019.0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>21.0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>1239</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5">
+        <v>41883.0</v>
+      </c>
+      <c r="B10" s="7">
+        <v>32428.0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>22.0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>1474</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5">
+        <v>41913.0</v>
+      </c>
+      <c r="B11" s="7">
+        <v>40204.0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>23.0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>1748</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5">
+        <v>41944.0</v>
+      </c>
+      <c r="B12" s="7">
+        <v>40400.0</v>
+      </c>
+      <c r="C12" s="7">
+        <v>20.0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>2020</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5">
+        <v>41974.0</v>
+      </c>
+      <c r="B13" s="7">
+        <v>50820.0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>22.0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>2310</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5">
+        <v>42005.0</v>
+      </c>
+      <c r="B14" s="7">
+        <v>54684.0</v>
+      </c>
+      <c r="C14" s="7">
+        <v>21.0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>2604</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5">
+        <v>42036.0</v>
+      </c>
+      <c r="B15" s="7">
+        <v>49708.0</v>
+      </c>
+      <c r="C15" s="7">
+        <v>17.0</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>2924</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5">
+        <v>42064.0</v>
+      </c>
+      <c r="B16" s="7">
+        <v>71632.0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>22.0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>3256</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>364</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5">
+        <v>42095.0</v>
+      </c>
+      <c r="B17" s="7">
+        <v>72400.0</v>
+      </c>
+      <c r="C17" s="7">
+        <v>20.0</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>3620</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5">
+        <v>42125.0</v>
+      </c>
+      <c r="B18" s="7">
+        <v>80000.0</v>
+      </c>
+      <c r="C18" s="7">
+        <v>20.0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>4000</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5">
+        <v>42156.0</v>
+      </c>
+      <c r="B19" s="7">
+        <v>92610.0</v>
+      </c>
+      <c r="C19" s="7">
+        <v>21.0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>4410</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5">
+        <v>42186.0</v>
+      </c>
+      <c r="B20" s="7">
+        <v>106480.0</v>
+      </c>
+      <c r="C20" s="7">
+        <v>22.0</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>4840</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5">
+        <v>42217.0</v>
+      </c>
+      <c r="B21" s="7">
+        <v>110691.0</v>
+      </c>
+      <c r="C21" s="7">
+        <v>21.0</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>5271</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5">
+        <v>42248.0</v>
+      </c>
+      <c r="B22" s="7">
+        <v>120393.0</v>
+      </c>
+      <c r="C22" s="7">
+        <v>21.0</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>5733</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>483</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5">
+        <v>42278.0</v>
+      </c>
+      <c r="B23" s="7">
+        <v>130536.0</v>
+      </c>
+      <c r="C23" s="7">
+        <v>21.0</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>6216</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5">
+        <v>42309.0</v>
+      </c>
+      <c r="B24" s="7">
+        <v>134000.0</v>
+      </c>
+      <c r="C24" s="7">
+        <v>20.0</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>6700</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>516</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5">
+        <v>42339.0</v>
+      </c>
+      <c r="B25" s="7">
+        <v>158752.0</v>
+      </c>
+      <c r="C25" s="7">
+        <v>22.0</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>7216</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="N27" s="10" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>